<commit_message>
Code rework to improve clarity and fix bugs
</commit_message>
<xml_diff>
--- a/SystemData/System_Specifications.xlsx
+++ b/SystemData/System_Specifications.xlsx
@@ -211,39 +211,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -499,7 +499,7 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -603,13 +603,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="6" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>0</v>
       </c>
       <c r="G2" s="6" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H2" s="7" t="n">
         <v>6</v>

</xml_diff>